<commit_message>
Added env config and scripts
</commit_message>
<xml_diff>
--- a/docs/sample_data copy.xlsx
+++ b/docs/sample_data copy.xlsx
@@ -62,7 +62,7 @@
     <t>结算日期</t>
   </si>
   <si>
-    <t>代理</t>
+    <t>业务经理</t>
   </si>
   <si>
     <t>电话</t>
@@ -5798,8 +5798,8 @@
   <sheetPr/>
   <dimension ref="A1:O358"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="D325" sqref="D325"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>

</xml_diff>